<commit_message>
Update room case setpoint configuration
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_OU44_room_case.xlsx
+++ b/twin4build/test/data/configuration_template_OU44_room_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64196074-FFDF-4EE4-84CF-B28B80160D13}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{532ADBA1-88FF-43FB-B3DE-1F6F8F925C03}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -379,12 +379,6 @@
     <t>visibleLightTransmittance</t>
   </si>
   <si>
-    <t>Heating meter</t>
-  </si>
-  <si>
-    <t>Space</t>
-  </si>
-  <si>
     <t>Co2</t>
   </si>
   <si>
@@ -406,21 +400,6 @@
     <t>Temperature controller</t>
   </si>
   <si>
-    <t>Valve position sensor</t>
-  </si>
-  <si>
-    <t>Damper position sensor</t>
-  </si>
-  <si>
-    <t>Space temperature sensor</t>
-  </si>
-  <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
     <t>CO2 controller</t>
   </si>
   <si>
@@ -430,7 +409,28 @@
     <t>Ø20-601b-2 temperature property;Ø20-601b-2 CO2 property</t>
   </si>
   <si>
-    <t>Space CO2 sensor</t>
+    <t>OE20-601b-2</t>
+  </si>
+  <si>
+    <t>OE20-601b-2| CO2 sensor</t>
+  </si>
+  <si>
+    <t>OE20-601b-2| temperature sensor</t>
+  </si>
+  <si>
+    <t>OE20-601b-2| Valve position sensor</t>
+  </si>
+  <si>
+    <t>OE20-601b-2| Damper position sensor</t>
+  </si>
+  <si>
+    <t>OE20-601b-2| Heating meter</t>
+  </si>
+  <si>
+    <t>Heating system</t>
+  </si>
+  <si>
+    <t>Ventilation system</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +982,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,46 +1108,46 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1181,12 +1181,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1211,16 +1211,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
         <v>96</v>
       </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>66</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>71</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>71</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>71</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>73</v>
@@ -1316,10 +1316,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>466.54</v>
@@ -1533,7 +1533,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,13 +1646,13 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
         <v>62</v>
@@ -1667,13 +1667,13 @@
         <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
         <v>63</v>
@@ -6694,8 +6694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F9D35B-B713-4EC3-BA55-A4EE8F2F331C}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6772,16 +6772,16 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L2">
         <f>(3*515+2*572)</f>
@@ -12747,8 +12747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070312A3-2F1C-41E0-AB34-E38166B9C92A}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12813,16 +12813,16 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G2">
         <f>5*0.468</f>
@@ -40279,7 +40279,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40309,30 +40309,30 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update util/load_speadsheet.py to use pandas datetime functions (renamed from load_file.py)
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_OU44_room_case.xlsx
+++ b/twin4build/test/data/configuration_template_OU44_room_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07FD0463-28B8-453F-ABC7-66A16D88467D}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59730C60-43CD-448C-B5C6-F79468B9A3DF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -1483,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88391AB-9A45-440E-B7CA-6D31485712DF}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747EB8B-49DD-40FE-8CAD-B5A7A33DF8B7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -6699,7 +6699,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12752,7 +12752,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add bypass LBNL test case
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_OU44_room_case.xlsx
+++ b/twin4build/test/data/configuration_template_OU44_room_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59730C60-43CD-448C-B5C6-F79468B9A3DF}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B00B8DAF-C206-4184-B474-981BB9B528F3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -659,10 +659,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1260,7 +1256,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,12 +1480,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1536,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747EB8B-49DD-40FE-8CAD-B5A7A33DF8B7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6699,7 +6695,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28197,7 +28193,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40283,7 +40279,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add changes for DP37 case study model
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_OU44_room_case.xlsx
+++ b/twin4build/test/data/configuration_template_OU44_room_case.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabj\OneDrive - Syddansk Universitet\PhD_Project_Jakob\Twin4build\python\BuildingEnergyModel\BuildingEnergyModel\twin4build\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{8660571A-4163-4FFB-91CA-F6ABE8F4478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B00B8DAF-C206-4184-B474-981BB9B528F3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E5FEDA-90C6-4BF6-8709-DFB39DA4EC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="count_name_occurences">_xlfn.LAMBDA(_xlpm.cell_,COUNTIF(ventilation_system_names,_xlpm.cell_)+COUNTIF(heating_system_names,_xlpm.cell_)+COUNTIF(cooling_system_names,_xlpm.cell_)+COUNTIF(damper_names,_xlpm.cell_)+COUNTIF(space_heater_names,_xlpm.cell_)+COUNTIF(valve_names,_xlpm.cell_)+COUNTIF(space_names,_xlpm.cell_)+COUNTIF(heating_coil_names,_xlpm.cell_)+COUNTIF(cooling_coil_names,_xlpm.cell_))</definedName>
     <definedName name="damper_names">OFFSET(Damper!$A$2, 0, 0, COUNTA(Damper!$A:$A), 1)</definedName>
     <definedName name="heating_coil_names">IF(COUNTA(Coil!$A:$A)&gt;1,OFFSET(Coil!$A$2, 0, 0, COUNTA(Coil!$A:$A), 1),"")</definedName>
-    <definedName name="heating_system_names">OFFSET(System!$B$2, 0, 0, COUNTA(System!$B:$B)-1, 1)</definedName>
+    <definedName name="heating_system_names">IF(COUNTA(System!$B:$B)&gt;1,OFFSET(System!$B$2, 0, 0, COUNTA(System!$B:$B)-1, 1),"")</definedName>
     <definedName name="property_class">named_ranges!$A$2:$A$1048576</definedName>
     <definedName name="property_instance">Property!$A$2:$A$1048576</definedName>
     <definedName name="sheet_dampers">Damper!$1:$1048576</definedName>
@@ -956,6 +956,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B0F6D5-8A47-48C4-A8B6-AFC37A61DB0A}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -996,6 +997,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C1460C-954B-4409-8D58-1A178EAA6542}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1074,6 +1076,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904F809-0565-4493-A542-77B590BDC86C}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1178,6 +1181,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E1EFB1-EA7C-414E-94A7-98027577BDF8}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1253,6 +1257,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDB24A9-A7F1-4854-93D9-EBD1381307DD}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1347,6 +1352,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D902D15-6209-46B5-9072-5070732D9943}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1446,6 +1452,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BFE67A-27F6-4BA1-B495-054A8677A66E}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1477,6 +1484,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88391AB-9A45-440E-B7CA-6D31485712DF}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1530,6 +1538,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747EB8B-49DD-40FE-8CAD-B5A7A33DF8B7}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6692,6 +6701,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F9D35B-B713-4EC3-BA55-A4EE8F2F331C}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12745,6 +12755,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070312A3-2F1C-41E0-AB34-E38166B9C92A}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22169,6 +22180,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B0EA7-434A-4CA3-97FE-A57E5232E2E7}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28190,6 +28202,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A142E3-535E-45D7-B544-7DE9118FD57D}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34242,6 +34255,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2999C7-12DB-42EA-8FDC-B5FA87CE6F00}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -40276,6 +40290,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EEF019-D7A4-42FF-B5C0-3702855A99F7}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>